<commit_message>
Updated Sensors sheet of Parts-list.xlsx
</commit_message>
<xml_diff>
--- a/Parts-list.xlsx
+++ b/Parts-list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Dirk/Documents/Work/Projects/Robotics/Handle/IG_Handle_hardware/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DC105EF3-AC19-EA45-8793-05B07B21E5C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0CFF14C-0844-224C-A58A-8495DAB7AB2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28960" yWindow="-4880" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28960" yWindow="-4880" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Digikey" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="179">
   <si>
     <t>The HTSUS and ECCN information shown is for informational purposes only and is not a representation or warranty as to the accuracy or reliability of these classifications. All information is provided "as is" and is subject to change without notice. Any use made of the information provided is without recourse to Digi-Key and at the user's risk.</t>
   </si>
@@ -556,6 +556,9 @@
   </si>
   <si>
     <t>Power and data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Socket Head Cap Screw, M5 x 0.8mm </t>
   </si>
 </sst>
 </file>
@@ -591,10 +594,10 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -911,7 +914,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2F3B7A0-E72D-C444-A817-885BAB36EAE3}">
   <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
@@ -1025,7 +1028,7 @@
       </c>
     </row>
     <row r="4" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>153</v>
       </c>
       <c r="B4" s="1">
@@ -1075,7 +1078,7 @@
       </c>
     </row>
     <row r="5" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="2"/>
+      <c r="A5" s="3"/>
       <c r="B5" s="1">
         <v>3</v>
       </c>
@@ -1123,7 +1126,7 @@
       </c>
     </row>
     <row r="6" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="2"/>
+      <c r="A6" s="3"/>
       <c r="B6" s="1">
         <v>4</v>
       </c>
@@ -1168,7 +1171,7 @@
       </c>
     </row>
     <row r="7" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="2"/>
+      <c r="A7" s="3"/>
       <c r="B7" s="1">
         <v>5</v>
       </c>
@@ -1213,7 +1216,7 @@
       </c>
     </row>
     <row r="8" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="3" t="s">
         <v>152</v>
       </c>
       <c r="B8" s="1">
@@ -1263,7 +1266,7 @@
       </c>
     </row>
     <row r="9" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="2"/>
+      <c r="A9" s="3"/>
       <c r="B9" s="1">
         <v>7</v>
       </c>
@@ -1311,7 +1314,7 @@
       </c>
     </row>
     <row r="10" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="2"/>
+      <c r="A10" s="3"/>
       <c r="B10" s="1">
         <v>8</v>
       </c>
@@ -1359,7 +1362,7 @@
       </c>
     </row>
     <row r="11" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="2"/>
+      <c r="A11" s="3"/>
       <c r="B11" s="1">
         <v>9</v>
       </c>
@@ -1407,7 +1410,7 @@
       </c>
     </row>
     <row r="12" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="2"/>
+      <c r="A12" s="3"/>
       <c r="B12" s="1">
         <v>10</v>
       </c>
@@ -1455,7 +1458,7 @@
       </c>
     </row>
     <row r="13" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="2"/>
+      <c r="A13" s="3"/>
       <c r="B13" s="1">
         <v>11</v>
       </c>
@@ -1553,7 +1556,7 @@
       </c>
     </row>
     <row r="15" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="3" t="s">
         <v>155</v>
       </c>
       <c r="B15" s="1">
@@ -1603,7 +1606,7 @@
       </c>
     </row>
     <row r="16" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="2"/>
+      <c r="A16" s="3"/>
       <c r="B16" s="1">
         <v>14</v>
       </c>
@@ -1648,7 +1651,7 @@
       </c>
     </row>
     <row r="17" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="2"/>
+      <c r="A17" s="3"/>
       <c r="B17" s="1">
         <v>15</v>
       </c>
@@ -1693,7 +1696,7 @@
       </c>
     </row>
     <row r="18" spans="1:16" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="3" t="s">
         <v>156</v>
       </c>
       <c r="B18" s="1">
@@ -1743,7 +1746,7 @@
       </c>
     </row>
     <row r="19" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="2"/>
+      <c r="A19" s="3"/>
       <c r="B19" s="1">
         <v>17</v>
       </c>
@@ -1791,7 +1794,7 @@
       </c>
     </row>
     <row r="20" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="2"/>
+      <c r="A20" s="3"/>
       <c r="B20" s="1">
         <v>18</v>
       </c>
@@ -1839,7 +1842,7 @@
       </c>
     </row>
     <row r="21" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="2"/>
+      <c r="A21" s="3"/>
       <c r="B21" s="1">
         <v>19</v>
       </c>
@@ -1906,94 +1909,105 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33A25E38-6294-7F43-BFFA-41D0180E850D}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>13084</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3" t="s">
+      <c r="C3" s="2"/>
+      <c r="D3" s="2" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="3">
+      <c r="A4" s="2">
         <v>4</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="3">
+      <c r="A5" s="2">
         <v>1</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="3">
+      <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>175</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>167</v>
+      </c>
+      <c r="D7" t="s">
+        <v>178</v>
       </c>
     </row>
   </sheetData>

</xml_diff>